<commit_message>
Update users and partners seed files
</commit_message>
<xml_diff>
--- a/lib/seeds/partners.xlsx
+++ b/lib/seeds/partners.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\smuca\smuca-web\lib\seeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61DC129A-1281-4E06-AEE3-2A054D506310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98F0B3E-CC54-4DC7-9E9B-19EBCF740E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{011C6046-B131-4BD8-A9DB-28C0EFA06D5A}"/>
+    <workbookView xWindow="6285" yWindow="3375" windowWidth="5790" windowHeight="10627" xr2:uid="{011C6046-B131-4BD8-A9DB-28C0EFA06D5A}"/>
   </bookViews>
   <sheets>
     <sheet name="partners" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>name</t>
   </si>
@@ -52,16 +52,34 @@
     <t>Clinique Saint-Amé</t>
   </si>
   <si>
-    <t>Clinique des 2 Caps</t>
-  </si>
-  <si>
-    <t>hpl.png</t>
-  </si>
-  <si>
     <t>ramsay_sante.png</t>
   </si>
   <si>
     <t>image/png</t>
+  </si>
+  <si>
+    <t>SOS Mains Côte d'Opale</t>
+  </si>
+  <si>
+    <t>sos_mains_cote_opale.jpg</t>
+  </si>
+  <si>
+    <t>vivalto_sante.jpg</t>
+  </si>
+  <si>
+    <t>image/jpg</t>
+  </si>
+  <si>
+    <t>Hôpital Chantilly Les Jockeys</t>
+  </si>
+  <si>
+    <t>hopital_chantilly_les_jockeys.png</t>
+  </si>
+  <si>
+    <t>Polyclinique Vauban</t>
+  </si>
+  <si>
+    <t>elsan.png</t>
   </si>
 </sst>
 </file>
@@ -117,8 +135,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9C59423-D1F1-4397-8677-FAA998EA84D0}" name="Table1" displayName="Table1" ref="A1:C4" totalsRowShown="0">
-  <autoFilter ref="A1:C4" xr:uid="{F9C59423-D1F1-4397-8677-FAA998EA84D0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F9C59423-D1F1-4397-8677-FAA998EA84D0}" name="Table1" displayName="Table1" ref="A1:C6" totalsRowShown="0">
+  <autoFilter ref="A1:C6" xr:uid="{F9C59423-D1F1-4397-8677-FAA998EA84D0}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{83A534BC-36A2-4EC0-969F-B60889DAAB3E}" name="name"/>
     <tableColumn id="2" xr3:uid="{7A217CB1-37C4-4CBA-B79D-C214251AB439}" name="logo_filename"/>
@@ -425,14 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEEF825E-A5B8-4DC9-BD53-6CF1852C1880}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="1" max="1" width="21.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.796875" customWidth="1"/>
     <col min="3" max="3" width="13.06640625" customWidth="1"/>
   </cols>
@@ -453,10 +472,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -464,21 +483,43 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CSV and Excel seed files
</commit_message>
<xml_diff>
--- a/lib/seeds/partners.xlsx
+++ b/lib/seeds/partners.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\smuca\smuca-web\lib\seeds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98F0B3E-CC54-4DC7-9E9B-19EBCF740E77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4F374F2-86A8-4E14-B5B2-6DE5E98A9CBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6285" yWindow="3375" windowWidth="5790" windowHeight="10627" xr2:uid="{011C6046-B131-4BD8-A9DB-28C0EFA06D5A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{011C6046-B131-4BD8-A9DB-28C0EFA06D5A}"/>
   </bookViews>
   <sheets>
     <sheet name="partners" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>name</t>
   </si>
@@ -61,15 +61,6 @@
     <t>SOS Mains Côte d'Opale</t>
   </si>
   <si>
-    <t>sos_mains_cote_opale.jpg</t>
-  </si>
-  <si>
-    <t>vivalto_sante.jpg</t>
-  </si>
-  <si>
-    <t>image/jpg</t>
-  </si>
-  <si>
     <t>Hôpital Chantilly Les Jockeys</t>
   </si>
   <si>
@@ -80,6 +71,12 @@
   </si>
   <si>
     <t>elsan.png</t>
+  </si>
+  <si>
+    <t>vivalto_sante.png</t>
+  </si>
+  <si>
+    <t>sos_mains_cote_opale.png</t>
   </si>
 </sst>
 </file>
@@ -446,7 +443,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -472,10 +469,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
@@ -491,10 +488,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -505,18 +502,18 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>

</xml_diff>